<commit_message>
clean-up of various files in repo
</commit_message>
<xml_diff>
--- a/notebook/200411/div_v_alignment_test1.xlsx
+++ b/notebook/200411/div_v_alignment_test1.xlsx
@@ -7,14 +7,15 @@
     <workbookView xWindow="240" yWindow="90" windowWidth="23505" windowHeight="10110"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Div_Align" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>mu</t>
   </si>
@@ -22,7 +23,13 @@
     <t>mu_count</t>
   </si>
   <si>
-    <t>align</t>
+    <t>bowtie2</t>
+  </si>
+  <si>
+    <t>sum</t>
+  </si>
+  <si>
+    <t>urmap</t>
   </si>
 </sst>
 </file>
@@ -100,11 +107,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Div_Align!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>align</c:v>
+                  <c:v>bowtie2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -116,7 +123,7 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>Div_Align!$B$2:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -158,7 +165,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$12</c:f>
+              <c:f>Div_Align!$C$2:$C$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="11"/>
@@ -194,6 +201,107 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>2.0500000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>urmap</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="7"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Div_Align!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Div_Align!$D$2:$D$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.61599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.25600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.114</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.9000000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.2999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.0000000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -201,7 +309,6 @@
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -209,11 +316,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="85380096"/>
-        <c:axId val="85378560"/>
+        <c:axId val="86420864"/>
+        <c:axId val="87654784"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="85380096"/>
+        <c:axId val="86420864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -249,12 +356,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85378560"/>
+        <c:crossAx val="87654784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="85378560"/>
+        <c:axId val="87654784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -287,10 +394,320 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85380096"/>
+        <c:crossAx val="86420864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Div_Align!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bowtie2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Div_Align!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Div_Align!$E$2:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>5.5390000000000006</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.6150000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.234</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.5650000000000004</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.504999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6110000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.587</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0290000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.66500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.49199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.44500000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Div_Align!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>urmap</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Div_Align!$B$2:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Div_Align!$F$2:$F$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.47499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.51600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.35</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.1380000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.77</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.585</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.5429999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5459999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.5129999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="151996672"/>
+        <c:axId val="152129536"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="151996672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="152129536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="152129536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Runtime</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="151996672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+      </c:dTable>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -308,16 +725,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>32095</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>25054</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>653291</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>41620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>16565</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>125067</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>546653</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>99391</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -331,6 +748,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>653499</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>115541</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>514351</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>108856</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -626,15 +1073,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" topLeftCell="G16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -644,8 +1091,17 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -656,8 +1112,17 @@
       <c r="C2" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>5.5390000000000006</v>
+      </c>
+      <c r="F2">
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>30</v>
       </c>
@@ -668,8 +1133,17 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <v>0.999</v>
+      </c>
+      <c r="E3">
+        <v>5.6150000000000002</v>
+      </c>
+      <c r="F3">
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>300</v>
       </c>
@@ -680,8 +1154,17 @@
       <c r="C4" s="1">
         <v>0.99990000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>0.998</v>
+      </c>
+      <c r="E4">
+        <v>6.234</v>
+      </c>
+      <c r="F4">
+        <v>1.2000000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1500</v>
       </c>
@@ -692,8 +1175,17 @@
       <c r="C5" s="1">
         <v>0.98029999999999995</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="E5">
+        <v>6.5650000000000004</v>
+      </c>
+      <c r="F5">
+        <v>6.67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3000</v>
       </c>
@@ -704,8 +1196,17 @@
       <c r="C6" s="1">
         <v>0.79359999999999997</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="E6">
+        <v>4.504999999999999</v>
+      </c>
+      <c r="F6">
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4500</v>
       </c>
@@ -716,8 +1217,17 @@
       <c r="C7" s="1">
         <v>0.54049999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="E7">
+        <v>2.6110000000000002</v>
+      </c>
+      <c r="F7">
+        <v>3.1380000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6000</v>
       </c>
@@ -728,8 +1238,17 @@
       <c r="C8" s="1">
         <v>0.34639999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>0.114</v>
+      </c>
+      <c r="E8">
+        <v>1.587</v>
+      </c>
+      <c r="F8">
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7500</v>
       </c>
@@ -740,8 +1259,17 @@
       <c r="C9" s="1">
         <v>0.20369999999999999</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="E9">
+        <v>1.0290000000000001</v>
+      </c>
+      <c r="F9">
+        <v>1.585</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9000</v>
       </c>
@@ -752,8 +1280,17 @@
       <c r="C10" s="1">
         <v>9.7100000000000006E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="F10">
+        <v>1.5429999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10500</v>
       </c>
@@ -764,8 +1301,17 @@
       <c r="C11" s="1">
         <v>3.6299999999999999E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E11">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="F11">
+        <v>1.5459999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12000</v>
       </c>
@@ -775,10 +1321,509 @@
       </c>
       <c r="C12" s="1">
         <v>2.0500000000000001E-2</v>
+      </c>
+      <c r="D12" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E12">
+        <v>0.44500000000000001</v>
+      </c>
+      <c r="F12">
+        <v>1.5129999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>2.6440000000000001</v>
+      </c>
+      <c r="D15">
+        <v>2.8519999999999999</v>
+      </c>
+      <c r="E15">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="F15">
+        <f>SUM(C15:E15)</f>
+        <v>5.5390000000000006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>30</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>2.6819999999999999</v>
+      </c>
+      <c r="D16">
+        <v>2.9079999999999999</v>
+      </c>
+      <c r="E16">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ref="F16:F25" si="1">SUM(C16:E16)</f>
+        <v>5.6150000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>300</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="C17">
+        <v>2.9860000000000002</v>
+      </c>
+      <c r="D17">
+        <v>3.1970000000000001</v>
+      </c>
+      <c r="E17">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>6.234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1500</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.98029999999999995</v>
+      </c>
+      <c r="C18">
+        <v>3.1480000000000001</v>
+      </c>
+      <c r="D18">
+        <v>3.3730000000000002</v>
+      </c>
+      <c r="E18">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="1"/>
+        <v>6.5650000000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3000</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0.79359999999999997</v>
+      </c>
+      <c r="C19">
+        <v>2.1419999999999999</v>
+      </c>
+      <c r="D19">
+        <v>2.34</v>
+      </c>
+      <c r="E19">
+        <v>2.3E-2</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>4.504999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4500</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.54049999999999998</v>
+      </c>
+      <c r="C20">
+        <v>1.224</v>
+      </c>
+      <c r="D20">
+        <v>1.36</v>
+      </c>
+      <c r="E20">
+        <v>2.7E-2</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="1"/>
+        <v>2.6110000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>6000</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0.34639999999999999</v>
+      </c>
+      <c r="C21">
+        <v>0.73899999999999999</v>
+      </c>
+      <c r="D21">
+        <v>0.84</v>
+      </c>
+      <c r="E21">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="1"/>
+        <v>1.587</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>7500</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0.20369999999999999</v>
+      </c>
+      <c r="C22">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="D22">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="E22">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="1"/>
+        <v>1.0290000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>9000</v>
+      </c>
+      <c r="B23" s="1">
+        <v>9.7100000000000006E-2</v>
+      </c>
+      <c r="C23">
+        <v>0.316</v>
+      </c>
+      <c r="D23">
+        <v>0.32100000000000001</v>
+      </c>
+      <c r="E23">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>0.66500000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>10500</v>
+      </c>
+      <c r="B24" s="1">
+        <v>3.6299999999999999E-2</v>
+      </c>
+      <c r="C24">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="D24">
+        <v>0.23699999999999999</v>
+      </c>
+      <c r="E24">
+        <v>1.9E-2</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>0.49199999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>12000</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2.0500000000000001E-2</v>
+      </c>
+      <c r="C25">
+        <v>0.216</v>
+      </c>
+      <c r="D25">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="E25">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>0.44500000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="F28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="D29">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="E29">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F29">
+        <f>SUM(C29:E29)</f>
+        <v>0.47499999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0.999</v>
+      </c>
+      <c r="C30">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="D30">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="E30">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F30">
+        <f t="shared" ref="F30:F39" si="2">SUM(C30:E30)</f>
+        <v>0.51600000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>300</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0.998</v>
+      </c>
+      <c r="C31">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="D31">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="E31">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="2"/>
+        <v>1.2000000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1500</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0.94</v>
+      </c>
+      <c r="C32">
+        <v>2.2280000000000002</v>
+      </c>
+      <c r="D32">
+        <v>4.4379999999999997</v>
+      </c>
+      <c r="E32">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="2"/>
+        <v>6.67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3000</v>
+      </c>
+      <c r="B33" s="1">
+        <v>0.61599999999999999</v>
+      </c>
+      <c r="C33">
+        <v>2.4550000000000001</v>
+      </c>
+      <c r="D33">
+        <v>4.891</v>
+      </c>
+      <c r="E33">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="2"/>
+        <v>7.35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>4500</v>
+      </c>
+      <c r="B34" s="1">
+        <v>0.25600000000000001</v>
+      </c>
+      <c r="C34">
+        <v>1.05</v>
+      </c>
+      <c r="D34">
+        <v>2.06</v>
+      </c>
+      <c r="E34">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="2"/>
+        <v>3.1380000000000003</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>6000</v>
+      </c>
+      <c r="B35" s="1">
+        <v>0.114</v>
+      </c>
+      <c r="C35">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="D35">
+        <v>1.1759999999999999</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="2"/>
+        <v>1.77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>7500</v>
+      </c>
+      <c r="B36" s="1">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="C36">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="D36">
+        <v>1.0489999999999999</v>
+      </c>
+      <c r="E36">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="2"/>
+        <v>1.585</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>9000</v>
+      </c>
+      <c r="B37" s="1">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C37">
+        <v>0.51800000000000002</v>
+      </c>
+      <c r="D37">
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="E37">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="2"/>
+        <v>1.5429999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>10500</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="C38">
+        <v>0.51900000000000002</v>
+      </c>
+      <c r="D38">
+        <v>1.0269999999999999</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="2"/>
+        <v>1.5459999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>12000</v>
+      </c>
+      <c r="B39" s="1">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C39">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="D39">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="2"/>
+        <v>1.5129999999999999</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>